<commit_message>
Entrega 2 de la primera iteración terminada, comienzo de código
</commit_message>
<xml_diff>
--- a/Actualizaciones.xlsx
+++ b/Actualizaciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumnosuaiedu-my.sharepoint.com/personal/ignacioadriel_roldanfarias_alumnos_uai_edu_ar/Documents/Desktop/Facu - copia/2025 1er cuatri/Proyecto/Primera Iteracion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{987020FF-DE03-4782-88B8-6128E2E8F658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{987020FF-DE03-4782-88B8-6128E2E8F658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3F0DC3A-A21B-4F8F-A7A6-7B1F70CA4221}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{D6BA3E01-E0E6-41CD-B1EF-ED32C0125CEC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Fecha</t>
   </si>
@@ -51,6 +51,45 @@
   </si>
   <si>
     <t>Requerimientos</t>
+  </si>
+  <si>
+    <t>Prototipos de interfaz de usuario</t>
+  </si>
+  <si>
+    <t>Autor</t>
+  </si>
+  <si>
+    <t>Ignacio Roldan</t>
+  </si>
+  <si>
+    <t>usuario cambiarlo por persona</t>
+  </si>
+  <si>
+    <t>visibilidad de los atributos, cambiarlos por privados</t>
+  </si>
+  <si>
+    <t>lista de rutinas dentro de cliente</t>
+  </si>
+  <si>
+    <t>lista de suscripción dentro de cliente</t>
+  </si>
+  <si>
+    <t>lista de progresos en el cliente</t>
+  </si>
+  <si>
+    <t>multiplicidad de ejercicio a ejercicio asignado(1 a 0..*)</t>
+  </si>
+  <si>
+    <t>Correcciones:</t>
+  </si>
+  <si>
+    <t>creación de una clase DiaRutina</t>
+  </si>
+  <si>
+    <t>Diagramas de secuencia core</t>
+  </si>
+  <si>
+    <t>Diagrama de clases</t>
   </si>
 </sst>
 </file>
@@ -107,6 +146,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -426,48 +469,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BED756E4-3BF9-407E-A807-57DE811657F5}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45782</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45787</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45797</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>45806</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>45824</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>45839</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>45843</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>45845</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>